<commit_message>
add two alg in <dp, match string>
</commit_message>
<xml_diff>
--- a/Doc/Questions_Journey/Questions_Journey.xlsx
+++ b/Doc/Questions_Journey/Questions_Journey.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\#project\ALGORITHM_Questions.Mars\Doc\Questions_Journey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DB8F819-2DC8-4E75-9DD9-0B738F571F48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6386DC88-B263-4319-8FFC-9684D1B76D6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="820" yWindow="-110" windowWidth="18490" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="25">
   <si>
     <t>LowestSales</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -114,6 +114,14 @@
   </si>
   <si>
     <t>√</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RegularExpressionMatching</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/regular-expression-matching/</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -202,11 +210,11 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -494,53 +502,53 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="6" topLeftCell="G1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G11" sqref="G11"/>
+      <selection pane="topRight" activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="1.75" customWidth="1"/>
     <col min="2" max="2" width="2.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.5" customWidth="1"/>
+    <col min="3" max="3" width="23.9140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.6640625" style="1"/>
     <col min="5" max="5" width="4" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="47.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="56.08203125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="14" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:14" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
     </row>
     <row r="3" spans="2:14" ht="15.5" x14ac:dyDescent="0.3">
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
       <c r="G3" s="2">
         <v>1</v>
       </c>
@@ -705,7 +713,7 @@
       <c r="B9" s="3">
         <v>6</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="5" t="s">
         <v>16</v>
       </c>
       <c r="D9" s="3" t="s">
@@ -732,14 +740,14 @@
       <c r="B10" s="3">
         <v>7</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="5" t="s">
         <v>20</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>17</v>
       </c>
       <c r="E10" s="3"/>
-      <c r="F10" s="7" t="s">
+      <c r="F10" s="6" t="s">
         <v>21</v>
       </c>
       <c r="G10" s="3" t="s">
@@ -754,12 +762,22 @@
       <c r="N10" s="3"/>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="3"/>
+      <c r="B11" s="3">
+        <v>8</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>17</v>
+      </c>
       <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
+      <c r="F11" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
@@ -1650,8 +1668,9 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="F10" r:id="rId1" xr:uid="{91248FDD-3F36-4DEE-8AAC-A1FA75681857}"/>
+    <hyperlink ref="F11" r:id="rId2" xr:uid="{42A599C5-0D5E-4656-AFAB-5BAC82764E1E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add Missing Number In Arithmetic Progression in Question_Journey.xlsx
</commit_message>
<xml_diff>
--- a/Doc/Questions_Journey/Questions_Journey.xlsx
+++ b/Doc/Questions_Journey/Questions_Journey.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\#project\ALGORITHM_Questions.Mars\Doc\Questions_Journey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6386DC88-B263-4319-8FFC-9684D1B76D6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDF87091-77E8-43BB-96B0-764C665B7C53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="820" yWindow="-110" windowWidth="18490" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="30">
   <si>
     <t>LowestSales</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -66,10 +66,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>real</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>screenshot</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -122,6 +118,30 @@
   </si>
   <si>
     <t>https://leetcode-cn.com/problems/regular-expression-matching/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MissingNumberInArithmeticProgression</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Math</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/missing-number-in-arithmetic-progression/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>√</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -502,16 +522,16 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="6" topLeftCell="G1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B11" sqref="B11"/>
+      <selection pane="topRight" activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="1.75" customWidth="1"/>
     <col min="2" max="2" width="2.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.9140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.08203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.6640625" style="1"/>
-    <col min="5" max="5" width="4" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="56.08203125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="14" width="8.6640625" style="1"/>
   </cols>
@@ -527,13 +547,13 @@
         <v>5</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="F2" s="7" t="s">
         <v>7</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>
@@ -584,14 +604,12 @@
       <c r="D4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="3"/>
+      <c r="F4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>15</v>
       </c>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
@@ -611,14 +629,12 @@
       <c r="D5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="3"/>
+      <c r="F5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>15</v>
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
@@ -638,14 +654,12 @@
       <c r="D6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>14</v>
-      </c>
+      <c r="E6" s="3"/>
       <c r="F6" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
@@ -665,14 +679,12 @@
       <c r="D7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="3" t="s">
-        <v>14</v>
-      </c>
+      <c r="E7" s="3"/>
       <c r="F7" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
@@ -692,14 +704,12 @@
       <c r="D8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>14</v>
-      </c>
+      <c r="E8" s="3"/>
       <c r="F8" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
@@ -714,19 +724,19 @@
         <v>6</v>
       </c>
       <c r="C9" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="E9" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F9" s="3" t="s">
+      <c r="G9" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>19</v>
       </c>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
@@ -741,17 +751,19 @@
         <v>7</v>
       </c>
       <c r="C10" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E10" s="3"/>
-      <c r="F10" s="6" t="s">
+      <c r="G10" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>22</v>
       </c>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
@@ -766,17 +778,19 @@
         <v>8</v>
       </c>
       <c r="C11" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E11" s="3"/>
-      <c r="F11" s="6" t="s">
-        <v>24</v>
-      </c>
       <c r="G11" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
@@ -787,12 +801,24 @@
       <c r="N11" s="3"/>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
+      <c r="B12" s="4">
+        <v>9</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>29</v>
+      </c>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
@@ -1669,8 +1695,9 @@
   <hyperlinks>
     <hyperlink ref="F10" r:id="rId1" xr:uid="{91248FDD-3F36-4DEE-8AAC-A1FA75681857}"/>
     <hyperlink ref="F11" r:id="rId2" xr:uid="{42A599C5-0D5E-4656-AFAB-5BAC82764E1E}"/>
+    <hyperlink ref="F12" r:id="rId3" xr:uid="{9F1C5CE1-D948-40B8-82DF-5CB83CEEF2EE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add longest valid parentheses
</commit_message>
<xml_diff>
--- a/Doc/Questions_Journey/Questions_Journey.xlsx
+++ b/Doc/Questions_Journey/Questions_Journey.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\#project\ALGORITHM_Questions.Mars\Doc\Questions_Journey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDF87091-77E8-43BB-96B0-764C665B7C53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C008C556-8B9D-449A-A342-2AFB5F95C660}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="820" yWindow="-110" windowWidth="18490" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="34">
   <si>
     <t>LowestSales</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -142,6 +142,22 @@
   </si>
   <si>
     <t>√</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LongestValidParentheses</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://leetcode-cn.com/problems/longest-valid-parentheses/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>×</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -522,13 +538,13 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="6" topLeftCell="G1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G13" sqref="G13"/>
+      <selection pane="topRight" activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="1.75" customWidth="1"/>
-    <col min="2" max="2" width="2.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="34.08203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.6640625" style="1"/>
     <col min="5" max="5" width="5.33203125" style="1" bestFit="1" customWidth="1"/>
@@ -828,12 +844,24 @@
       <c r="N12" s="3"/>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
+      <c r="B13" s="4">
+        <v>10</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>33</v>
+      </c>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
@@ -1696,8 +1724,9 @@
     <hyperlink ref="F10" r:id="rId1" xr:uid="{91248FDD-3F36-4DEE-8AAC-A1FA75681857}"/>
     <hyperlink ref="F11" r:id="rId2" xr:uid="{42A599C5-0D5E-4656-AFAB-5BAC82764E1E}"/>
     <hyperlink ref="F12" r:id="rId3" xr:uid="{9F1C5CE1-D948-40B8-82DF-5CB83CEEF2EE}"/>
+    <hyperlink ref="F13" r:id="rId4" xr:uid="{656B3792-0751-4B6F-AD5D-2F76FC895177}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>